<commit_message>
Formatted graphs in plant analysis
</commit_message>
<xml_diff>
--- a/Lab3/DataAndCalculations/PlantMath2.xlsx
+++ b/Lab3/DataAndCalculations/PlantMath2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willk\Documents\MECHA4\MECH423\Lab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liam_\Documents\University\4th Year\2022W\MECH 423\Willem\MECH423\Lab3\DataAndCalculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8597C2E0-35C4-4B35-BFFA-A56059323BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CFBCFA-22EC-4E67-AE17-602C50B00CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{F626948C-F66D-40EC-9D0C-34C1D19506D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{F626948C-F66D-40EC-9D0C-34C1D19506D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="5" r:id="rId1"/>
@@ -216,6 +216,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Steady-state</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Encoder Speed vs PWM Duty Cycle</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -287,6 +317,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.147025371828521E-2"/>
+                  <c:y val="0.25421296296296297"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Calculations!$A$3:$A$6</c:f>
@@ -368,6 +448,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>PWM Duty Cycle [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -430,6 +565,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Encoder</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Speed [counts/s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -690,6 +885,36 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -752,6 +977,36 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2334,7 +2589,7 @@
   <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2720,7 +2975,7 @@
   <dimension ref="A1:N693"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>